<commit_message>
OS: compare codes as strings, leading zeros (Vendor + Customer); output 2302
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/output/2302/Reconciliation_Ekofisk.xlsx
+++ b/output/2302/Reconciliation_Ekofisk.xlsx
@@ -26404,7 +26404,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>0004</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -26426,7 +26426,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>0011</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -26448,7 +26448,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>107</t>
+          <t>0015</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -26470,7 +26470,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>0032</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -26492,7 +26492,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>0033</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -26514,7 +26514,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>0039</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -26536,7 +26536,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>0063</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -26558,7 +26558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>0068</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -26580,11 +26580,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>118</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
+          <t>0070</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>X</t>
@@ -26594,7 +26602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>119</t>
+          <t>0071</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -26616,11 +26624,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
+          <t>0072</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>X</t>
@@ -26630,7 +26646,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>0073</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -26652,7 +26668,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>0080</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -26674,7 +26690,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>0083</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -26696,11 +26712,19 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>127-4737</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
+          <t>0085</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>X</t>
@@ -26710,11 +26734,19 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>130-8311</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
+          <t>0096</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr">
         <is>
           <t>X</t>
@@ -26724,7 +26756,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>139-7736</t>
+          <t>0098</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -26738,7 +26770,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>0104</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -26760,7 +26792,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>0105</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -26782,11 +26814,19 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>166-0471</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
+          <t>0107</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr">
         <is>
           <t>X</t>
@@ -26796,11 +26836,19 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>166-2899</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
+          <t>0109</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr">
         <is>
           <t>X</t>
@@ -26810,11 +26858,19 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>168-7250</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
+          <t>0110</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D23" t="inlineStr">
         <is>
           <t>X</t>
@@ -26824,7 +26880,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>170-2992</t>
+          <t>0115</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -26846,7 +26902,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>182-7179</t>
+          <t>0117</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -26868,7 +26924,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>202-2416</t>
+          <t>0118</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -26882,7 +26938,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>202583</t>
+          <t>0119</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -26890,31 +26946,47 @@
           <t>X</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>202593</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>0120</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>204-0954</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr"/>
+          <t>0121</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D29" t="inlineStr">
         <is>
           <t>X</t>
@@ -26924,7 +26996,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>209933</t>
+          <t>0123</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -26937,12 +27009,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>215978</t>
+          <t>0125</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -26964,7 +27040,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>216-6577</t>
+          <t>0156</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -26986,37 +27062,25 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>220330</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr"/>
+          <t>127-4737</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>220475</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>130-8311</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
           <t>X</t>
@@ -27026,7 +27090,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>221-1555</t>
+          <t>139-7736</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -27040,25 +27104,21 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>221345</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr"/>
+          <t>166-0471</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>232-4887</t>
+          <t>166-2899</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -27072,7 +27132,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>233-6659</t>
+          <t>168-7250</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -27086,7 +27146,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>236-3919</t>
+          <t>170-2992</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -27108,11 +27168,19 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>250-5683</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr"/>
-      <c r="C40" t="inlineStr"/>
+          <t>182-7179</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D40" t="inlineStr">
         <is>
           <t>X</t>
@@ -27122,19 +27190,11 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>260-5426</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>202-2416</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr">
         <is>
           <t>X</t>
@@ -27144,47 +27204,39 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>265-3806</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr"/>
+          <t>202583</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="D42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>280-1843</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr"/>
+          <t>202593</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="D43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>281-9068</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>204-0954</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr">
         <is>
           <t>X</t>
@@ -27194,25 +27246,37 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>282-4647</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>209933</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>284-5352</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr"/>
+          <t>215978</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D46" t="inlineStr">
         <is>
           <t>X</t>
@@ -27222,7 +27286,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>284-5378</t>
+          <t>216-6577</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -27244,25 +27308,37 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>286-1508</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr"/>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>220330</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>286-3082</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr"/>
+          <t>220475</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D49" t="inlineStr">
         <is>
           <t>X</t>
@@ -27272,7 +27348,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>299-0869</t>
+          <t>221-1555</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -27286,7 +27362,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>314-7196</t>
+          <t>221345</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -27299,28 +27375,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="D51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>232-4887</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr">
         <is>
           <t>X</t>
@@ -27330,19 +27394,11 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>325-7367</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>233-6659</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
           <t>X</t>
@@ -27352,7 +27408,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>328-8453</t>
+          <t>236-3919</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -27374,19 +27430,11 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>250-5683</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
           <t>X</t>
@@ -27396,11 +27444,19 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>348-9986</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr"/>
+          <t>260-5426</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D56" t="inlineStr">
         <is>
           <t>X</t>
@@ -27410,7 +27466,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>349-2170</t>
+          <t>265-3806</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -27424,19 +27480,11 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>352-0301</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>280-1843</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr">
         <is>
           <t>X</t>
@@ -27446,11 +27494,19 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>360-8494</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr"/>
+          <t>281-9068</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D59" t="inlineStr">
         <is>
           <t>X</t>
@@ -27460,19 +27516,11 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>362-5506</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>282-4647</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
           <t>X</t>
@@ -27482,19 +27530,11 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>3680</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>284-5352</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
           <t>X</t>
@@ -27504,11 +27544,19 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>369-4866</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr"/>
-      <c r="C62" t="inlineStr"/>
+          <t>284-5378</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D62" t="inlineStr">
         <is>
           <t>X</t>
@@ -27518,19 +27566,11 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>384-5104</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>286-1508</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
           <t>X</t>
@@ -27540,19 +27580,11 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>39</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>286-3082</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr">
         <is>
           <t>X</t>
@@ -27562,19 +27594,11 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>299-0869</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
           <t>X</t>
@@ -27584,11 +27608,19 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>400-7845</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr"/>
-      <c r="C66" t="inlineStr"/>
+          <t>314-7196</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D66" t="inlineStr">
         <is>
           <t>X</t>
@@ -27598,11 +27630,19 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>429-9335</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr"/>
-      <c r="C67" t="inlineStr"/>
+          <t>325-7367</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D67" t="inlineStr">
         <is>
           <t>X</t>
@@ -27612,7 +27652,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>431-2849</t>
+          <t>328-8453</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -27634,19 +27674,11 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>437-3205</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>348-9986</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr">
         <is>
           <t>X</t>
@@ -27656,7 +27688,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>441-5592</t>
+          <t>349-2170</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -27670,11 +27702,19 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>446-8377</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr"/>
-      <c r="C71" t="inlineStr"/>
+          <t>352-0301</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D71" t="inlineStr">
         <is>
           <t>X</t>
@@ -27684,7 +27724,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>446-8492</t>
+          <t>360-8494</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -27698,11 +27738,19 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>457-2129</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr"/>
-      <c r="C73" t="inlineStr"/>
+          <t>362-5506</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D73" t="inlineStr">
         <is>
           <t>X</t>
@@ -27712,7 +27760,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>470-9465</t>
+          <t>3680</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -27734,7 +27782,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>473-5825</t>
+          <t>369-4866</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -27748,11 +27796,19 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>5008-8707</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr"/>
-      <c r="C76" t="inlineStr"/>
+          <t>384-5104</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D76" t="inlineStr">
         <is>
           <t>X</t>
@@ -27762,7 +27818,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>501-6175</t>
+          <t>400-7845</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
@@ -27776,7 +27832,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>5010-9198</t>
+          <t>429-9335</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
@@ -27790,11 +27846,19 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>501112-3014</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr"/>
-      <c r="C79" t="inlineStr"/>
+          <t>431-2849</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D79" t="inlineStr">
         <is>
           <t>X</t>
@@ -27804,7 +27868,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>5035-7995</t>
+          <t>437-3205</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -27826,19 +27890,11 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>5040-1058</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>441-5592</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr">
         <is>
           <t>X</t>
@@ -27848,7 +27904,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>5043-5726</t>
+          <t>446-8377</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
@@ -27862,7 +27918,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>5051-6822</t>
+          <t>446-8492</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
@@ -27876,19 +27932,11 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>5054-6845</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>457-2129</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr">
         <is>
           <t>X</t>
@@ -27898,7 +27946,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>5070-3826</t>
+          <t>470-9465</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -27920,7 +27968,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>5077-3530</t>
+          <t>473-5825</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
@@ -27934,7 +27982,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>5080-7403</t>
+          <t>5008-8707</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -27948,19 +27996,11 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>5086-1962</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>501-6175</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
         <is>
           <t>X</t>
@@ -27970,19 +28010,11 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>5086-6557</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5010-9198</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr">
         <is>
           <t>X</t>
@@ -27992,7 +28024,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>5095-1771</t>
+          <t>501112-3014</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
@@ -28006,11 +28038,19 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>511-6272</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr"/>
-      <c r="C91" t="inlineStr"/>
+          <t>5035-7995</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D91" t="inlineStr">
         <is>
           <t>X</t>
@@ -28020,11 +28060,19 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>5132-9464</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr"/>
-      <c r="C92" t="inlineStr"/>
+          <t>5040-1058</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D92" t="inlineStr">
         <is>
           <t>X</t>
@@ -28034,7 +28082,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>514-7806</t>
+          <t>5043-5726</t>
         </is>
       </c>
       <c r="B93" t="inlineStr"/>
@@ -28048,7 +28096,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>5141-8341</t>
+          <t>5051-6822</t>
         </is>
       </c>
       <c r="B94" t="inlineStr"/>
@@ -28062,11 +28110,19 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>5155-4020</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr"/>
+          <t>5054-6845</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D95" t="inlineStr">
         <is>
           <t>X</t>
@@ -28076,7 +28132,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>5160-9543</t>
+          <t>5070-3826</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -28098,7 +28154,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>5161-2893</t>
+          <t>5077-3530</t>
         </is>
       </c>
       <c r="B97" t="inlineStr"/>
@@ -28112,7 +28168,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>5162-1183</t>
+          <t>5080-7403</t>
         </is>
       </c>
       <c r="B98" t="inlineStr"/>
@@ -28126,11 +28182,19 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>5163-5795</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr"/>
-      <c r="C99" t="inlineStr"/>
+          <t>5086-1962</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D99" t="inlineStr">
         <is>
           <t>X</t>
@@ -28140,11 +28204,19 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>5169-1319</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr"/>
-      <c r="C100" t="inlineStr"/>
+          <t>5086-6557</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D100" t="inlineStr">
         <is>
           <t>X</t>
@@ -28154,7 +28226,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>5188-5994</t>
+          <t>5095-1771</t>
         </is>
       </c>
       <c r="B101" t="inlineStr"/>
@@ -28168,19 +28240,11 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>5205-1588</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>511-6272</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="inlineStr"/>
       <c r="D102" t="inlineStr">
         <is>
           <t>X</t>
@@ -28190,19 +28254,11 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>5206-0456</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5132-9464</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="inlineStr"/>
       <c r="D103" t="inlineStr">
         <is>
           <t>X</t>
@@ -28212,7 +28268,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>523-4745</t>
+          <t>514-7806</t>
         </is>
       </c>
       <c r="B104" t="inlineStr"/>
@@ -28226,19 +28282,11 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>5237-9310</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5141-8341</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr">
         <is>
           <t>X</t>
@@ -28248,7 +28296,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>5238-6661</t>
+          <t>5155-4020</t>
         </is>
       </c>
       <c r="B106" t="inlineStr"/>
@@ -28262,11 +28310,19 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>5238-9954</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr"/>
-      <c r="C107" t="inlineStr"/>
+          <t>5160-9543</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D107" t="inlineStr">
         <is>
           <t>X</t>
@@ -28276,7 +28332,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>5247-2032</t>
+          <t>5161-2893</t>
         </is>
       </c>
       <c r="B108" t="inlineStr"/>
@@ -28290,7 +28346,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>5247-6777</t>
+          <t>5162-1183</t>
         </is>
       </c>
       <c r="B109" t="inlineStr"/>
@@ -28304,19 +28360,11 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>527-1960</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5163-5795</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr"/>
       <c r="D110" t="inlineStr">
         <is>
           <t>X</t>
@@ -28326,7 +28374,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>5287-3312</t>
+          <t>5169-1319</t>
         </is>
       </c>
       <c r="B111" t="inlineStr"/>
@@ -28340,7 +28388,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>5328-4428-1</t>
+          <t>5188-5994</t>
         </is>
       </c>
       <c r="B112" t="inlineStr"/>
@@ -28354,11 +28402,19 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>5329-3460</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr"/>
-      <c r="C113" t="inlineStr"/>
+          <t>5205-1588</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D113" t="inlineStr">
         <is>
           <t>X</t>
@@ -28368,11 +28424,19 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>5338-8757</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr"/>
-      <c r="C114" t="inlineStr"/>
+          <t>5206-0456</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D114" t="inlineStr">
         <is>
           <t>X</t>
@@ -28382,19 +28446,11 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>5341-9354</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>523-4745</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" t="inlineStr"/>
       <c r="D115" t="inlineStr">
         <is>
           <t>X</t>
@@ -28404,11 +28460,19 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>5374-5105</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr"/>
-      <c r="C116" t="inlineStr"/>
+          <t>5237-9310</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D116" t="inlineStr">
         <is>
           <t>X</t>
@@ -28418,7 +28482,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>5398-3052</t>
+          <t>5238-6661</t>
         </is>
       </c>
       <c r="B117" t="inlineStr"/>
@@ -28432,19 +28496,11 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>541-1731</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5238-9954</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr"/>
+      <c r="C118" t="inlineStr"/>
       <c r="D118" t="inlineStr">
         <is>
           <t>X</t>
@@ -28454,19 +28510,11 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>5412-6941</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5247-2032</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr"/>
+      <c r="C119" t="inlineStr"/>
       <c r="D119" t="inlineStr">
         <is>
           <t>X</t>
@@ -28476,19 +28524,11 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>5415-8779</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5247-6777</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr"/>
+      <c r="C120" t="inlineStr"/>
       <c r="D120" t="inlineStr">
         <is>
           <t>X</t>
@@ -28498,7 +28538,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>5432-8364</t>
+          <t>527-1960</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -28520,19 +28560,11 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>5445-2230</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5287-3312</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr"/>
+      <c r="C122" t="inlineStr"/>
       <c r="D122" t="inlineStr">
         <is>
           <t>X</t>
@@ -28542,7 +28574,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>5451-0656</t>
+          <t>5328-4428-1</t>
         </is>
       </c>
       <c r="B123" t="inlineStr"/>
@@ -28556,19 +28588,11 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>5469-2413</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5329-3460</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr"/>
+      <c r="C124" t="inlineStr"/>
       <c r="D124" t="inlineStr">
         <is>
           <t>X</t>
@@ -28578,19 +28602,11 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>5475-9816</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5338-8757</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr"/>
+      <c r="C125" t="inlineStr"/>
       <c r="D125" t="inlineStr">
         <is>
           <t>X</t>
@@ -28600,11 +28616,19 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>5484-9559</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr"/>
-      <c r="C126" t="inlineStr"/>
+          <t>5341-9354</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D126" t="inlineStr">
         <is>
           <t>X</t>
@@ -28614,7 +28638,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>5493-6125</t>
+          <t>5374-5105</t>
         </is>
       </c>
       <c r="B127" t="inlineStr"/>
@@ -28628,19 +28652,11 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>5493-7016</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5398-3052</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr"/>
+      <c r="C128" t="inlineStr"/>
       <c r="D128" t="inlineStr">
         <is>
           <t>X</t>
@@ -28650,7 +28666,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>5500-2117</t>
+          <t>541-1731</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -28672,7 +28688,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>551-0367</t>
+          <t>5412-6941</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -28694,11 +28710,19 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>5518-1374</t>
-        </is>
-      </c>
-      <c r="B131" t="inlineStr"/>
-      <c r="C131" t="inlineStr"/>
+          <t>5415-8779</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D131" t="inlineStr">
         <is>
           <t>X</t>
@@ -28708,11 +28732,19 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>5522-2798</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr"/>
-      <c r="C132" t="inlineStr"/>
+          <t>5432-8364</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D132" t="inlineStr">
         <is>
           <t>X</t>
@@ -28722,11 +28754,19 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>5525-9345</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr"/>
-      <c r="C133" t="inlineStr"/>
+          <t>5445-2230</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D133" t="inlineStr">
         <is>
           <t>X</t>
@@ -28736,7 +28776,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>5529-0977</t>
+          <t>5451-0656</t>
         </is>
       </c>
       <c r="B134" t="inlineStr"/>
@@ -28750,11 +28790,19 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>5542-8130</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr"/>
-      <c r="C135" t="inlineStr"/>
+          <t>5469-2413</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D135" t="inlineStr">
         <is>
           <t>X</t>
@@ -28764,11 +28812,19 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>556490-6716</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr"/>
-      <c r="C136" t="inlineStr"/>
+          <t>5475-9816</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D136" t="inlineStr">
         <is>
           <t>X</t>
@@ -28778,7 +28834,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>5569548950</t>
+          <t>5484-9559</t>
         </is>
       </c>
       <c r="B137" t="inlineStr"/>
@@ -28792,7 +28848,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>5617-0483</t>
+          <t>5493-6125</t>
         </is>
       </c>
       <c r="B138" t="inlineStr"/>
@@ -28806,11 +28862,19 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>5622-2714</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr"/>
-      <c r="C139" t="inlineStr"/>
+          <t>5493-7016</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D139" t="inlineStr">
         <is>
           <t>X</t>
@@ -28820,7 +28884,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>5632-1169</t>
+          <t>5500-2117</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -28842,11 +28906,19 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>5636-9838</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr"/>
-      <c r="C141" t="inlineStr"/>
+          <t>551-0367</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D141" t="inlineStr">
         <is>
           <t>X</t>
@@ -28856,19 +28928,11 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>5645-5785</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5518-1374</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr"/>
+      <c r="C142" t="inlineStr"/>
       <c r="D142" t="inlineStr">
         <is>
           <t>X</t>
@@ -28878,7 +28942,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>5648-2664</t>
+          <t>5522-2798</t>
         </is>
       </c>
       <c r="B143" t="inlineStr"/>
@@ -28892,19 +28956,11 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>5665-2324</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5525-9345</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr"/>
+      <c r="C144" t="inlineStr"/>
       <c r="D144" t="inlineStr">
         <is>
           <t>X</t>
@@ -28914,7 +28970,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>5675-3346</t>
+          <t>5529-0977</t>
         </is>
       </c>
       <c r="B145" t="inlineStr"/>
@@ -28928,7 +28984,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>569-5259</t>
+          <t>5542-8130</t>
         </is>
       </c>
       <c r="B146" t="inlineStr"/>
@@ -28942,7 +28998,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>5707-9055</t>
+          <t>556490-6716</t>
         </is>
       </c>
       <c r="B147" t="inlineStr"/>
@@ -28956,7 +29012,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>5711-5487</t>
+          <t>5569548950</t>
         </is>
       </c>
       <c r="B148" t="inlineStr"/>
@@ -28970,7 +29026,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>572-7748</t>
+          <t>5617-0483</t>
         </is>
       </c>
       <c r="B149" t="inlineStr"/>
@@ -28984,19 +29040,11 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>5747-9172</t>
-        </is>
-      </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5622-2714</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr"/>
+      <c r="C150" t="inlineStr"/>
       <c r="D150" t="inlineStr">
         <is>
           <t>X</t>
@@ -29006,7 +29054,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>5750-3260</t>
+          <t>5632-1169</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -29028,19 +29076,11 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>5751-8466</t>
-        </is>
-      </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5636-9838</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr"/>
+      <c r="C152" t="inlineStr"/>
       <c r="D152" t="inlineStr">
         <is>
           <t>X</t>
@@ -29050,7 +29090,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>5755-3802</t>
+          <t>5645-5785</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -29072,7 +29112,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>576-9021</t>
+          <t>5648-2664</t>
         </is>
       </c>
       <c r="B154" t="inlineStr"/>
@@ -29086,11 +29126,19 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>5762-5675</t>
-        </is>
-      </c>
-      <c r="B155" t="inlineStr"/>
-      <c r="C155" t="inlineStr"/>
+          <t>5665-2324</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D155" t="inlineStr">
         <is>
           <t>X</t>
@@ -29100,19 +29148,11 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>5771-2770</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5675-3346</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr"/>
+      <c r="C156" t="inlineStr"/>
       <c r="D156" t="inlineStr">
         <is>
           <t>X</t>
@@ -29122,7 +29162,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>578-0275</t>
+          <t>569-5259</t>
         </is>
       </c>
       <c r="B157" t="inlineStr"/>
@@ -29136,7 +29176,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>5806-4411</t>
+          <t>5707-9055</t>
         </is>
       </c>
       <c r="B158" t="inlineStr"/>
@@ -29150,19 +29190,11 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>5828-6345</t>
-        </is>
-      </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5711-5487</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr"/>
+      <c r="C159" t="inlineStr"/>
       <c r="D159" t="inlineStr">
         <is>
           <t>X</t>
@@ -29172,7 +29204,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>5839-4040</t>
+          <t>572-7748</t>
         </is>
       </c>
       <c r="B160" t="inlineStr"/>
@@ -29186,11 +29218,19 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>5851-3797</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr"/>
-      <c r="C161" t="inlineStr"/>
+          <t>5747-9172</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D161" t="inlineStr">
         <is>
           <t>X</t>
@@ -29200,11 +29240,19 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>5872-4170</t>
-        </is>
-      </c>
-      <c r="B162" t="inlineStr"/>
-      <c r="C162" t="inlineStr"/>
+          <t>5750-3260</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D162" t="inlineStr">
         <is>
           <t>X</t>
@@ -29214,11 +29262,19 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>5888-3406</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr"/>
-      <c r="C163" t="inlineStr"/>
+          <t>5751-8466</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D163" t="inlineStr">
         <is>
           <t>X</t>
@@ -29228,11 +29284,19 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>590-3927</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr"/>
-      <c r="C164" t="inlineStr"/>
+          <t>5755-3802</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D164" t="inlineStr">
         <is>
           <t>X</t>
@@ -29242,7 +29306,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>5911-6871</t>
+          <t>576-9021</t>
         </is>
       </c>
       <c r="B165" t="inlineStr"/>
@@ -29256,19 +29320,11 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>5916-3113</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5762-5675</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr"/>
+      <c r="C166" t="inlineStr"/>
       <c r="D166" t="inlineStr">
         <is>
           <t>X</t>
@@ -29278,11 +29334,19 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>5921-4759</t>
-        </is>
-      </c>
-      <c r="B167" t="inlineStr"/>
-      <c r="C167" t="inlineStr"/>
+          <t>5771-2770</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D167" t="inlineStr">
         <is>
           <t>X</t>
@@ -29292,19 +29356,11 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>5927-8374</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>578-0275</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr"/>
+      <c r="C168" t="inlineStr"/>
       <c r="D168" t="inlineStr">
         <is>
           <t>X</t>
@@ -29314,19 +29370,11 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>5933-2668</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5806-4411</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr"/>
+      <c r="C169" t="inlineStr"/>
       <c r="D169" t="inlineStr">
         <is>
           <t>X</t>
@@ -29336,7 +29384,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>5944-5734</t>
+          <t>5828-6345</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -29358,7 +29406,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>5951-3044</t>
+          <t>5839-4040</t>
         </is>
       </c>
       <c r="B171" t="inlineStr"/>
@@ -29372,7 +29420,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>5957-9052</t>
+          <t>5851-3797</t>
         </is>
       </c>
       <c r="B172" t="inlineStr"/>
@@ -29386,7 +29434,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>5975-3673</t>
+          <t>5872-4170</t>
         </is>
       </c>
       <c r="B173" t="inlineStr"/>
@@ -29400,19 +29448,11 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>5976-4233</t>
-        </is>
-      </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C174" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5888-3406</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr"/>
+      <c r="C174" t="inlineStr"/>
       <c r="D174" t="inlineStr">
         <is>
           <t>X</t>
@@ -29422,7 +29462,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>5986-1039</t>
+          <t>590-3927</t>
         </is>
       </c>
       <c r="B175" t="inlineStr"/>
@@ -29436,7 +29476,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>5987-3968</t>
+          <t>5911-6871</t>
         </is>
       </c>
       <c r="B176" t="inlineStr"/>
@@ -29450,11 +29490,19 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>5990-3443</t>
-        </is>
-      </c>
-      <c r="B177" t="inlineStr"/>
-      <c r="C177" t="inlineStr"/>
+          <t>5916-3113</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D177" t="inlineStr">
         <is>
           <t>X</t>
@@ -29464,7 +29512,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>5991-1321</t>
+          <t>5921-4759</t>
         </is>
       </c>
       <c r="B178" t="inlineStr"/>
@@ -29478,7 +29526,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>600-6514</t>
+          <t>5927-8374</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -29500,11 +29548,19 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>603-3922</t>
-        </is>
-      </c>
-      <c r="B180" t="inlineStr"/>
-      <c r="C180" t="inlineStr"/>
+          <t>5933-2668</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D180" t="inlineStr">
         <is>
           <t>X</t>
@@ -29514,7 +29570,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>608-1327</t>
+          <t>5944-5734</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -29536,19 +29592,11 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>615-5725</t>
-        </is>
-      </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C182" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5951-3044</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr"/>
+      <c r="C182" t="inlineStr"/>
       <c r="D182" t="inlineStr">
         <is>
           <t>X</t>
@@ -29558,7 +29606,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>620-5280</t>
+          <t>5957-9052</t>
         </is>
       </c>
       <c r="B183" t="inlineStr"/>
@@ -29572,19 +29620,11 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>624-2028</t>
-        </is>
-      </c>
-      <c r="B184" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C184" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>5975-3673</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr"/>
+      <c r="C184" t="inlineStr"/>
       <c r="D184" t="inlineStr">
         <is>
           <t>X</t>
@@ -29594,7 +29634,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>5976-4233</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -29616,7 +29656,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>645-8558</t>
+          <t>5986-1039</t>
         </is>
       </c>
       <c r="B186" t="inlineStr"/>
@@ -29630,7 +29670,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>649-4470</t>
+          <t>5987-3968</t>
         </is>
       </c>
       <c r="B187" t="inlineStr"/>
@@ -29644,7 +29684,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>661-1073</t>
+          <t>5990-3443</t>
         </is>
       </c>
       <c r="B188" t="inlineStr"/>
@@ -29658,7 +29698,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>664-9396</t>
+          <t>5991-1321</t>
         </is>
       </c>
       <c r="B189" t="inlineStr"/>
@@ -29672,11 +29712,19 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>666-9626</t>
-        </is>
-      </c>
-      <c r="B190" t="inlineStr"/>
-      <c r="C190" t="inlineStr"/>
+          <t>600-6514</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D190" t="inlineStr">
         <is>
           <t>X</t>
@@ -29686,19 +29734,11 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>68</t>
-        </is>
-      </c>
-      <c r="B191" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C191" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>603-3922</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr"/>
+      <c r="C191" t="inlineStr"/>
       <c r="D191" t="inlineStr">
         <is>
           <t>X</t>
@@ -29708,11 +29748,19 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>681-3794</t>
-        </is>
-      </c>
-      <c r="B192" t="inlineStr"/>
-      <c r="C192" t="inlineStr"/>
+          <t>608-1327</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D192" t="inlineStr">
         <is>
           <t>X</t>
@@ -29722,11 +29770,19 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>685-9847</t>
-        </is>
-      </c>
-      <c r="B193" t="inlineStr"/>
-      <c r="C193" t="inlineStr"/>
+          <t>615-5725</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D193" t="inlineStr">
         <is>
           <t>X</t>
@@ -29736,19 +29792,11 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>698-4678</t>
-        </is>
-      </c>
-      <c r="B194" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C194" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>620-5280</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr"/>
+      <c r="C194" t="inlineStr"/>
       <c r="D194" t="inlineStr">
         <is>
           <t>X</t>
@@ -29758,11 +29806,19 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>699-9858</t>
-        </is>
-      </c>
-      <c r="B195" t="inlineStr"/>
-      <c r="C195" t="inlineStr"/>
+          <t>624-2028</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D195" t="inlineStr">
         <is>
           <t>X</t>
@@ -29772,19 +29828,11 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>70</t>
-        </is>
-      </c>
-      <c r="B196" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C196" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>645-8558</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr"/>
+      <c r="C196" t="inlineStr"/>
       <c r="D196" t="inlineStr">
         <is>
           <t>X</t>
@@ -29794,7 +29842,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>700-1761</t>
+          <t>649-4470</t>
         </is>
       </c>
       <c r="B197" t="inlineStr"/>
@@ -29808,7 +29856,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>704-5537</t>
+          <t>661-1073</t>
         </is>
       </c>
       <c r="B198" t="inlineStr"/>
@@ -29822,19 +29870,11 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>71</t>
-        </is>
-      </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C199" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>664-9396</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr"/>
+      <c r="C199" t="inlineStr"/>
       <c r="D199" t="inlineStr">
         <is>
           <t>X</t>
@@ -29844,19 +29884,11 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>72</t>
-        </is>
-      </c>
-      <c r="B200" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C200" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>666-9626</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr"/>
+      <c r="C200" t="inlineStr"/>
       <c r="D200" t="inlineStr">
         <is>
           <t>X</t>
@@ -29866,7 +29898,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>724-5707</t>
+          <t>681-3794</t>
         </is>
       </c>
       <c r="B201" t="inlineStr"/>
@@ -29880,19 +29912,11 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>73</t>
-        </is>
-      </c>
-      <c r="B202" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C202" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>685-9847</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr"/>
+      <c r="C202" t="inlineStr"/>
       <c r="D202" t="inlineStr">
         <is>
           <t>X</t>
@@ -29902,7 +29926,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>731-2861</t>
+          <t>698-4678</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -29924,7 +29948,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>733-1838</t>
+          <t>699-9858</t>
         </is>
       </c>
       <c r="B204" t="inlineStr"/>
@@ -29938,7 +29962,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>734-6232</t>
+          <t>700-1761</t>
         </is>
       </c>
       <c r="B205" t="inlineStr"/>
@@ -29952,7 +29976,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>734-8618</t>
+          <t>704-5537</t>
         </is>
       </c>
       <c r="B206" t="inlineStr"/>
@@ -29966,19 +29990,11 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>735-2297</t>
-        </is>
-      </c>
-      <c r="B207" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C207" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>724-5707</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr"/>
+      <c r="C207" t="inlineStr"/>
       <c r="D207" t="inlineStr">
         <is>
           <t>X</t>
@@ -29988,7 +30004,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>747-0842</t>
+          <t>731-2861</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -30010,7 +30026,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>750-6454</t>
+          <t>733-1838</t>
         </is>
       </c>
       <c r="B209" t="inlineStr"/>
@@ -30024,7 +30040,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>757-1227</t>
+          <t>734-6232</t>
         </is>
       </c>
       <c r="B210" t="inlineStr"/>
@@ -30038,19 +30054,11 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>769-8079</t>
-        </is>
-      </c>
-      <c r="B211" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C211" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>734-8618</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr"/>
+      <c r="C211" t="inlineStr"/>
       <c r="D211" t="inlineStr">
         <is>
           <t>X</t>
@@ -30060,11 +30068,19 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>796-1097</t>
-        </is>
-      </c>
-      <c r="B212" t="inlineStr"/>
-      <c r="C212" t="inlineStr"/>
+          <t>735-2297</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D212" t="inlineStr">
         <is>
           <t>X</t>
@@ -30074,11 +30090,19 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>797-2466</t>
-        </is>
-      </c>
-      <c r="B213" t="inlineStr"/>
-      <c r="C213" t="inlineStr"/>
+          <t>747-0842</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D213" t="inlineStr">
         <is>
           <t>X</t>
@@ -30088,19 +30112,11 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>80</t>
-        </is>
-      </c>
-      <c r="B214" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C214" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>750-6454</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr"/>
+      <c r="C214" t="inlineStr"/>
       <c r="D214" t="inlineStr">
         <is>
           <t>X</t>
@@ -30110,7 +30126,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>801-4896</t>
+          <t>757-1227</t>
         </is>
       </c>
       <c r="B215" t="inlineStr"/>
@@ -30124,11 +30140,19 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>811-4092</t>
-        </is>
-      </c>
-      <c r="B216" t="inlineStr"/>
-      <c r="C216" t="inlineStr"/>
+          <t>769-8079</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D216" t="inlineStr">
         <is>
           <t>X</t>
@@ -30138,7 +30162,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>811-7442</t>
+          <t>796-1097</t>
         </is>
       </c>
       <c r="B217" t="inlineStr"/>
@@ -30152,19 +30176,11 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>820-9256</t>
-        </is>
-      </c>
-      <c r="B218" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C218" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>797-2466</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr"/>
+      <c r="C218" t="inlineStr"/>
       <c r="D218" t="inlineStr">
         <is>
           <t>X</t>
@@ -30174,7 +30190,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>824-3586</t>
+          <t>801-4896</t>
         </is>
       </c>
       <c r="B219" t="inlineStr"/>
@@ -30188,19 +30204,11 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>83</t>
-        </is>
-      </c>
-      <c r="B220" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C220" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>811-4092</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr"/>
+      <c r="C220" t="inlineStr"/>
       <c r="D220" t="inlineStr">
         <is>
           <t>X</t>
@@ -30210,7 +30218,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>831-2332</t>
+          <t>811-7442</t>
         </is>
       </c>
       <c r="B221" t="inlineStr"/>
@@ -30224,11 +30232,19 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>834-4384</t>
-        </is>
-      </c>
-      <c r="B222" t="inlineStr"/>
-      <c r="C222" t="inlineStr"/>
+          <t>820-9256</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D222" t="inlineStr">
         <is>
           <t>X</t>
@@ -30238,7 +30254,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>842-3972</t>
+          <t>824-3586</t>
         </is>
       </c>
       <c r="B223" t="inlineStr"/>
@@ -30252,19 +30268,11 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>847-6269</t>
-        </is>
-      </c>
-      <c r="B224" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C224" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>831-2332</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr"/>
+      <c r="C224" t="inlineStr"/>
       <c r="D224" t="inlineStr">
         <is>
           <t>X</t>
@@ -30274,19 +30282,11 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>85</t>
-        </is>
-      </c>
-      <c r="B225" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C225" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>834-4384</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr"/>
+      <c r="C225" t="inlineStr"/>
       <c r="D225" t="inlineStr">
         <is>
           <t>X</t>
@@ -30296,7 +30296,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>853-1121</t>
+          <t>842-3972</t>
         </is>
       </c>
       <c r="B226" t="inlineStr"/>
@@ -30310,7 +30310,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>859-5753</t>
+          <t>847-6269</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -30332,19 +30332,11 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>865-6928</t>
-        </is>
-      </c>
-      <c r="B228" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C228" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>853-1121</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr"/>
+      <c r="C228" t="inlineStr"/>
       <c r="D228" t="inlineStr">
         <is>
           <t>X</t>
@@ -30354,11 +30346,19 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>867-4046</t>
-        </is>
-      </c>
-      <c r="B229" t="inlineStr"/>
-      <c r="C229" t="inlineStr"/>
+          <t>859-5753</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D229" t="inlineStr">
         <is>
           <t>X</t>
@@ -30368,11 +30368,19 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>886-6691</t>
-        </is>
-      </c>
-      <c r="B230" t="inlineStr"/>
-      <c r="C230" t="inlineStr"/>
+          <t>865-6928</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D230" t="inlineStr">
         <is>
           <t>X</t>
@@ -30382,7 +30390,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>890-4906</t>
+          <t>867-4046</t>
         </is>
       </c>
       <c r="B231" t="inlineStr"/>
@@ -30396,7 +30404,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>896301-9</t>
+          <t>886-6691</t>
         </is>
       </c>
       <c r="B232" t="inlineStr"/>
@@ -30410,19 +30418,11 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>939-5385</t>
-        </is>
-      </c>
-      <c r="B233" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C233" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>890-4906</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr"/>
+      <c r="C233" t="inlineStr"/>
       <c r="D233" t="inlineStr">
         <is>
           <t>X</t>
@@ -30432,7 +30432,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>939-8884</t>
+          <t>896301-9</t>
         </is>
       </c>
       <c r="B234" t="inlineStr"/>
@@ -30446,11 +30446,19 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>945-1170</t>
-        </is>
-      </c>
-      <c r="B235" t="inlineStr"/>
-      <c r="C235" t="inlineStr"/>
+          <t>939-5385</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D235" t="inlineStr">
         <is>
           <t>X</t>
@@ -30460,19 +30468,11 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="B236" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C236" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>939-8884</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr"/>
+      <c r="C236" t="inlineStr"/>
       <c r="D236" t="inlineStr">
         <is>
           <t>X</t>
@@ -30482,19 +30482,11 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>968-3186</t>
-        </is>
-      </c>
-      <c r="B237" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C237" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>945-1170</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr"/>
+      <c r="C237" t="inlineStr"/>
       <c r="D237" t="inlineStr">
         <is>
           <t>X</t>
@@ -30504,11 +30496,19 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="B238" t="inlineStr"/>
-      <c r="C238" t="inlineStr"/>
+          <t>968-3186</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D238" t="inlineStr">
         <is>
           <t>X</t>

</xml_diff>